<commit_message>
Modified product landing sheet
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_productlanding.xlsx
+++ b/docs/OVW Sheets/OVWDemo_productlanding.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agarnepu\Desktop\Nov-23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration Dec 9\OVWMigration\docs\OVW Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ja_jp" sheetId="48" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1696" uniqueCount="441">
   <si>
     <t>http://www.cisco.com/web/ANZ/products/telepresence/index.html</t>
   </si>
@@ -1385,6 +1385,15 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/UA/uk/solutions/collaboration/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/solucoes/datacenter/index.html​</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/solucoes/collaboration/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/BR/solucoes/borderless/index.html</t>
   </si>
 </sst>
 </file>
@@ -1423,7 +1432,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1433,6 +1442,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1465,7 +1480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1473,6 +1488,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1756,7 +1778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -8486,8 +8508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8596,8 +8618,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>69</v>
+      <c r="A8" s="7" t="s">
+        <v>438</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -8610,8 +8632,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>70</v>
+      <c r="A9" s="8" t="s">
+        <v>440</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -8624,8 +8646,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>71</v>
+      <c r="A10" s="9" t="s">
+        <v>439</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
@@ -8639,18 +8661,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1"/>
-    <hyperlink ref="A9" r:id="rId2"/>
-    <hyperlink ref="A10" r:id="rId3"/>
-    <hyperlink ref="A1" r:id="rId4"/>
-    <hyperlink ref="A2" r:id="rId5"/>
-    <hyperlink ref="A3" r:id="rId6"/>
-    <hyperlink ref="A4" r:id="rId7"/>
-    <hyperlink ref="A5" r:id="rId8"/>
-    <hyperlink ref="A6" r:id="rId9"/>
-    <hyperlink ref="A7" r:id="rId10"/>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId6"/>
+    <hyperlink ref="A7" r:id="rId7"/>
+    <hyperlink ref="A8" r:id="rId8" display="http://www.cisco.com/web/BR/solucoes/datacenter/index.html"/>
+    <hyperlink ref="A9" r:id="rId9"/>
+    <hyperlink ref="A10" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>